<commit_message>
Changed K3 and other stuff
</commit_message>
<xml_diff>
--- a/Lab0x05/on_pc/IMU verifier.xlsx
+++ b/Lab0x05/on_pc/IMU verifier.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Documents\GitHub\ME-405-Repo\Lab0x05\on_pc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathe\Documents\GitHub\ME-405-Repo\Lab0x05\on_pc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4A1716EA-7C91-486B-AD99-053B9085C310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96587C17-7E72-4BC7-8C16-0ACB05713F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F3D89DD9-DBC1-45AF-8745-14C71D4CA817}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{F3D89DD9-DBC1-45AF-8745-14C71D4CA817}"/>
   </bookViews>
   <sheets>
     <sheet name="IMU verifier" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>time_micros</t>
   </si>
@@ -38,6 +51,9 @@
   </si>
   <si>
     <t>angle accumulate</t>
+  </si>
+  <si>
+    <t>Average Yaw Rate</t>
   </si>
 </sst>
 </file>
@@ -658,166 +674,163 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>0.73002089999999997</c:v>
+                  <c:v>0.100232</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74001830000000002</c:v>
+                  <c:v>0.100232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7499789</c:v>
+                  <c:v>0.300284</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76005409999999995</c:v>
+                  <c:v>0.40082899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76993549999999999</c:v>
+                  <c:v>0.50031599999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.77995950000000003</c:v>
+                  <c:v>0.60033800000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7899969</c:v>
+                  <c:v>0.70072400000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.79994109999999996</c:v>
+                  <c:v>0.80023</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80996990000000002</c:v>
+                  <c:v>0.90079299999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.81999659999999996</c:v>
+                  <c:v>0.90079299999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.82995509999999995</c:v>
+                  <c:v>1.0018119999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.83999679999999999</c:v>
+                  <c:v>1.200251</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84995690000000002</c:v>
+                  <c:v>1.3003290000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.85999460000000005</c:v>
+                  <c:v>1.4002410000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.87003459999999999</c:v>
+                  <c:v>1.5002260000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.87999190000000005</c:v>
+                  <c:v>1.5002260000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.88996379999999997</c:v>
+                  <c:v>1.7007890000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.89998199999999995</c:v>
+                  <c:v>1.8008789999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.91000709999999996</c:v>
+                  <c:v>1.900234</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.92001520000000003</c:v>
+                  <c:v>2.000486</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.92999869999999996</c:v>
+                  <c:v>2.1005479999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.94003389999999998</c:v>
+                  <c:v>2.1005479999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.94998930000000004</c:v>
+                  <c:v>2.300694</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.96003070000000001</c:v>
+                  <c:v>2.400541</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.96997460000000002</c:v>
+                  <c:v>2.500562</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.98000330000000002</c:v>
+                  <c:v>2.6006649999999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.98996490000000004</c:v>
+                  <c:v>2.7008369999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99985369999999996</c:v>
+                  <c:v>2.8004099999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.0099913</c:v>
+                  <c:v>2.8004099999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.0199444</c:v>
+                  <c:v>3.0002080000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0299885</c:v>
+                  <c:v>3.0002080000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.039965</c:v>
+                  <c:v>3.1018029999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.0499559000000001</c:v>
+                  <c:v>3.3119459999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.0599940999999999</c:v>
+                  <c:v>3.4005740000000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.0700308000000001</c:v>
+                  <c:v>3.5003739999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.079996</c:v>
+                  <c:v>3.6006200000000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.0899581</c:v>
+                  <c:v>3.7003460000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.0999858</c:v>
+                  <c:v>3.8005230000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.1099412</c:v>
+                  <c:v>3.9007580000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.1199737000000001</c:v>
+                  <c:v>4.0007780000000004</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.1300136000000001</c:v>
+                  <c:v>4.0007780000000004</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.1400154</c:v>
+                  <c:v>4.2005699999999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.1500372999999999</c:v>
+                  <c:v>4.3008069999999998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.1600511</c:v>
+                  <c:v>4.4003899999999998</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.1699215000000001</c:v>
+                  <c:v>4.5005519999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.1799693</c:v>
+                  <c:v>4.6003920000000003</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.1899913</c:v>
+                  <c:v>4.700672</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.1999192000000001</c:v>
+                  <c:v>4.80063</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.2099815</c:v>
+                  <c:v>4.900709</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.2200139000000001</c:v>
+                  <c:v>5.0005750000000004</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.2299788</c:v>
+                  <c:v>5.1005669999999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.2399538999999999</c:v>
+                  <c:v>5.2006160000000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.250024</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.2599834000000001</c:v>
+                  <c:v>5.3007390000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,166 +842,163 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>4.6166669999999996</c:v>
+                  <c:v>5.5233340000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6175223335554394</c:v>
+                  <c:v>5.5233340000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6170409047878538</c:v>
+                  <c:v>5.5236674199666584</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6171640461340608</c:v>
+                  <c:v>5.5233322699499006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6171860048034725</c:v>
+                  <c:v>5.5229453760499574</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5841513553588085</c:v>
+                  <c:v>5.9586523049407365</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5141572176859084</c:v>
+                  <c:v>0.6124029642991502</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4509563026828083</c:v>
+                  <c:v>1.4847941566311502</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.4066290066828078</c:v>
+                  <c:v>2.11443026212415</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.3682713093509582</c:v>
+                  <c:v>2.11443026212415</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.3258591682237082</c:v>
+                  <c:v>2.58747981290615</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.2849169280663082</c:v>
+                  <c:v>3.4485949392611501</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.2466535455596581</c:v>
+                  <c:v>3.8632514692741506</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.2071830807902577</c:v>
+                  <c:v>4.252741715970151</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.1686294807902575</c:v>
+                  <c:v>4.6239637743076507</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.1309742879711573</c:v>
+                  <c:v>4.6239637743076507</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.0924384338616075</c:v>
+                  <c:v>5.3726209283216511</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0547533065313077</c:v>
+                  <c:v>5.7552427783416507</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.0175156289743574</c:v>
+                  <c:v>6.1283208033416514</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.9806413399739071</c:v>
+                  <c:v>0.2054857461760653</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.9443513174739073</c:v>
+                  <c:v>0.57243536397106487</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.9068865691347074</c:v>
+                  <c:v>0.57243536397106487</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.8693215248088073</c:v>
+                  <c:v>1.3164225784560655</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.8327708288088074</c:v>
+                  <c:v>1.6785898134900656</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.7975417986546072</c:v>
+                  <c:v>2.0419438518175652</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.7609370436546072</c:v>
+                  <c:v>2.3961972573845647</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.7245550689794071</c:v>
+                  <c:v>2.752197426292565</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.6887136622078076</c:v>
+                  <c:v>3.1262046668955645</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.6510412153342071</c:v>
+                  <c:v>3.1262046668955645</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.6140654488342072</c:v>
+                  <c:v>3.8710072557395661</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.5777504428146072</c:v>
+                  <c:v>3.8710072557395661</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.5419514336518572</c:v>
+                  <c:v>4.2408130557395651</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.5055068534271072</c:v>
+                  <c:v>5.0219612384855647</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.4676572632070077</c:v>
+                  <c:v>5.3451579970475658</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.4300976986412572</c:v>
+                  <c:v>5.6999469970475642</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.3947267743098575</c:v>
+                  <c:v>6.0699104738235654</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.3590347865771073</c:v>
+                  <c:v>0.15931262209297881</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.3225952378518073</c:v>
+                  <c:v>0.5353103121224787</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.2865732805259076</c:v>
+                  <c:v>0.91158137603747891</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.2500048180259071</c:v>
+                  <c:v>1.2705420538174796</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.2133536058614571</c:v>
+                  <c:v>1.2705420538174796</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.1772915608615575</c:v>
+                  <c:v>1.995010022729478</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.1407673025270078</c:v>
+                  <c:v>2.3591487409969778</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.1033323785247076</c:v>
+                  <c:v>2.7183667294229776</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.0663622425823074</c:v>
+                  <c:v>3.080229749377978</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.0296263654526077</c:v>
+                  <c:v>3.4395982383379793</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.9938756615576079</c:v>
+                  <c:v>3.806957271577978</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.9582841400576076</c:v>
+                  <c:v>4.1744695015849782</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.9210089081652577</c:v>
+                  <c:v>4.5416482438159784</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.8837608341580574</c:v>
+                  <c:v>4.9089332215639798</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.8472117931658576</c:v>
+                  <c:v>5.2720152726759775</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.8103316290061078</c:v>
+                  <c:v>5.6316358504564787</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.7731673660655574</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>2.7371032731721572</c:v>
+                  <c:v>6.0023690921504782</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1025,166 +1035,163 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>0.73002089999999997</c:v>
+                  <c:v>0.100232</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.74001830000000002</c:v>
+                  <c:v>0.100232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.7499789</c:v>
+                  <c:v>0.300284</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.76005409999999995</c:v>
+                  <c:v>0.40082899999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.76993549999999999</c:v>
+                  <c:v>0.50031599999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.77995950000000003</c:v>
+                  <c:v>0.60033800000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.7899969</c:v>
+                  <c:v>0.70072400000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.79994109999999996</c:v>
+                  <c:v>0.80023</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.80996990000000002</c:v>
+                  <c:v>0.90079299999999995</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.81999659999999996</c:v>
+                  <c:v>0.90079299999999995</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.82995509999999995</c:v>
+                  <c:v>1.0018119999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.83999679999999999</c:v>
+                  <c:v>1.200251</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.84995690000000002</c:v>
+                  <c:v>1.3003290000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.85999460000000005</c:v>
+                  <c:v>1.4002410000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.87003459999999999</c:v>
+                  <c:v>1.5002260000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.87999190000000005</c:v>
+                  <c:v>1.5002260000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.88996379999999997</c:v>
+                  <c:v>1.7007890000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.89998199999999995</c:v>
+                  <c:v>1.8008789999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.91000709999999996</c:v>
+                  <c:v>1.900234</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.92001520000000003</c:v>
+                  <c:v>2.000486</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.92999869999999996</c:v>
+                  <c:v>2.1005479999999999</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.94003389999999998</c:v>
+                  <c:v>2.1005479999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.94998930000000004</c:v>
+                  <c:v>2.300694</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.96003070000000001</c:v>
+                  <c:v>2.400541</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.96997460000000002</c:v>
+                  <c:v>2.500562</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.98000330000000002</c:v>
+                  <c:v>2.6006649999999998</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.98996490000000004</c:v>
+                  <c:v>2.7008369999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.99985369999999996</c:v>
+                  <c:v>2.8004099999999998</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.0099913</c:v>
+                  <c:v>2.8004099999999998</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.0199444</c:v>
+                  <c:v>3.0002080000000002</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.0299885</c:v>
+                  <c:v>3.0002080000000002</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.039965</c:v>
+                  <c:v>3.1018029999999999</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.0499559000000001</c:v>
+                  <c:v>3.3119459999999998</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.0599940999999999</c:v>
+                  <c:v>3.4005740000000002</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.0700308000000001</c:v>
+                  <c:v>3.5003739999999999</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.079996</c:v>
+                  <c:v>3.6006200000000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.0899581</c:v>
+                  <c:v>3.7003460000000001</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.0999858</c:v>
+                  <c:v>3.8005230000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.1099412</c:v>
+                  <c:v>3.9007580000000002</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.1199737000000001</c:v>
+                  <c:v>4.0007780000000004</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.1300136000000001</c:v>
+                  <c:v>4.0007780000000004</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.1400154</c:v>
+                  <c:v>4.2005699999999999</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.1500372999999999</c:v>
+                  <c:v>4.3008069999999998</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.1600511</c:v>
+                  <c:v>4.4003899999999998</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.1699215000000001</c:v>
+                  <c:v>4.5005519999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.1799693</c:v>
+                  <c:v>4.6003920000000003</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.1899913</c:v>
+                  <c:v>4.700672</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.1999192000000001</c:v>
+                  <c:v>4.80063</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.2099815</c:v>
+                  <c:v>4.900709</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.2200139000000001</c:v>
+                  <c:v>5.0005750000000004</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.2299788</c:v>
+                  <c:v>5.1005669999999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.2399538999999999</c:v>
+                  <c:v>5.2006160000000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.250024</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>1.2599834000000001</c:v>
+                  <c:v>5.3007390000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1196,166 +1203,163 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>4.6166669999999996</c:v>
+                  <c:v>5.5233340000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6011110000000004</c:v>
+                  <c:v>5.5233340000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6022220000000003</c:v>
+                  <c:v>5.5233340000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6022220000000003</c:v>
+                  <c:v>5.5233340000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.6022220000000003</c:v>
+                  <c:v>5.5233340000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.88</c:v>
+                  <c:v>5.8611110000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.572222</c:v>
+                  <c:v>0.51111119999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.1644439999999996</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28444439999999999</c:v>
+                  <c:v>2.0477780000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.64444449999999998</c:v>
+                  <c:v>2.0477780000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.0511109999999999</c:v>
+                  <c:v>2.423333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4388890000000001</c:v>
+                  <c:v>3.2455560000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8011109999999999</c:v>
+                  <c:v>3.6422219999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.1755550000000001</c:v>
+                  <c:v>4.0122220000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.5511110000000001</c:v>
+                  <c:v>4.3633329999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
+                  <c:v>4.3633329999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.0766669999999996</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.4377779999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.7977780000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.14</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.24444440000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.24444440000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.92222219999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.263333</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.611111</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.947778</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.2844440000000001</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.6433330000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.6433330000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.342222</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.342222</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.4288889999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.7033329999999998</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.0422219999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.39</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.7444439999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.0944440000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.17222219999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.51444440000000002</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.51444440000000002</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.2144440000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.562222</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.9044449999999999</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.5911110000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>2.943333</c:v>
                 </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.2766670000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.637778</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.9944440000000001</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>4.3411109999999997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.6822220000000003</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.032222</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.3911110000000004</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.7711110000000003</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>6.0733329999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.1366667</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.48333330000000002</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.82555559999999995</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1.1822220000000001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>1.5377780000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>1.8833329999999999</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>2.2255560000000001</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.5733329999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>2.9344440000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.2966669999999998</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.6677780000000002</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.9377779999999998</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>4.29</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4.6355560000000002</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>4.9822220000000002</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>5.3288890000000002</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>5.6733330000000004</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>6.016667</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>0.1244444</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.1244444</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.79222219999999999</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.131111</c:v>
-                </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.4744440000000001</c:v>
+                  <c:v>3.3277779999999999</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.828889</c:v>
+                  <c:v>3.641111</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.1844440000000001</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.5311110000000001</c:v>
+                  <c:v>4.3355560000000004</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.8844439999999998</c:v>
+                  <c:v>4.6722219999999997</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.2388889999999999</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>3.585556</c:v>
+                  <c:v>5.0244450000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2114,16 +2118,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>489584</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>52386</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>284479</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>101599</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2468,18 +2472,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482207D4-79B3-4978-9DD7-F10B8042D38D}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2499,1188 +2509,1232 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>7300209</v>
+        <v>100232</v>
       </c>
       <c r="B2">
-        <v>4.6166669999999996</v>
+        <v>5.5233340000000002</v>
       </c>
       <c r="C2">
-        <v>0.28555560000000002</v>
+        <v>-3.333333E-3</v>
       </c>
       <c r="D2">
-        <v>0.73002089999999997</v>
+        <f>A2/1000000</f>
+        <v>0.100232</v>
       </c>
       <c r="F2">
         <f>B2</f>
-        <v>4.6166669999999996</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.5233340000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7400183</v>
+        <v>100232</v>
       </c>
       <c r="B3">
-        <v>4.6011110000000004</v>
+        <v>5.5233340000000002</v>
       </c>
       <c r="C3">
-        <v>-0.1144444</v>
+        <v>-3.333333E-3</v>
       </c>
       <c r="D3">
-        <v>0.74001830000000002</v>
+        <f t="shared" ref="D3:D54" si="0">A3/1000000</f>
+        <v>0.100232</v>
       </c>
       <c r="E3">
         <f>0.5*(C3+C2)*(D3-D2)</f>
-        <v>8.55333555440004E-4</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f>MOD(E3+F2, 2*PI())</f>
-        <v>4.6175223335554394</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.5233340000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>7499789</v>
+        <v>300284</v>
       </c>
       <c r="B4">
-        <v>4.6022220000000003</v>
+        <v>5.5233340000000002</v>
       </c>
       <c r="C4">
-        <v>1.777778E-2</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.7499789</v>
+        <f t="shared" si="0"/>
+        <v>0.300284</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E55" si="0">0.5*(C4+C3)*(D4-D3)</f>
-        <v>-4.8142876758599937E-4</v>
+        <f>-0.5*(C4+C3)*(D4-D3)</f>
+        <v>3.3341996665800001E-4</v>
       </c>
       <c r="F4">
         <f>MOD(E4+F3, 2*PI())</f>
-        <v>4.6170409047878538</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5.5236674199666584</v>
+      </c>
+      <c r="I4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>7600541</v>
+        <v>400829</v>
       </c>
       <c r="B5">
-        <v>4.6022220000000003</v>
+        <v>5.5233340000000002</v>
       </c>
       <c r="C5">
         <v>6.6666670000000003E-3</v>
       </c>
       <c r="D5">
-        <v>0.76005409999999995</v>
+        <f t="shared" si="0"/>
+        <v>0.40082899999999999</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1.2314134620719942E-4</v>
+        <f t="shared" ref="E5:E55" si="1">-0.5*(C5+C4)*(D5-D4)</f>
+        <v>-3.351500167575E-4</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F55" si="1">MOD(E5+F4, 2*PI())</f>
-        <v>4.6171640461340608</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F5:F55" si="2">MOD(E5+F4, 2*PI())</f>
+        <v>5.5233322699499006</v>
+      </c>
+      <c r="I5">
+        <f>AVERAGE(C2:C54)</f>
+        <v>-3.691740054490567</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>7699355</v>
+        <v>500316</v>
       </c>
       <c r="B6">
-        <v>4.6022220000000003</v>
+        <v>5.5233340000000002</v>
       </c>
       <c r="C6">
-        <v>-2.2222219999999998E-3</v>
+        <v>1.1111109999999999E-3</v>
       </c>
       <c r="D6">
-        <v>0.76993549999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.50031599999999998</v>
       </c>
       <c r="E6">
-        <f t="shared" si="0"/>
-        <v>2.195866941150009E-5</v>
+        <f t="shared" si="1"/>
+        <v>-3.8689389994299997E-4</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
-        <v>4.6171860048034725</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>5.5229453760499574</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>7799595</v>
+        <v>600338</v>
       </c>
       <c r="B7">
-        <v>4.88</v>
+        <v>5.8611110000000002</v>
       </c>
       <c r="C7">
-        <v>-6.588889</v>
+        <v>-8.7133330000000004</v>
       </c>
       <c r="D7">
-        <v>0.77995950000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.60033800000000004</v>
       </c>
       <c r="E7">
-        <f t="shared" si="0"/>
-        <v>-3.303464944466411E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.43570692889077928</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
-        <v>4.5841513553588085</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>5.9586523049407365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7899969</v>
+        <v>700724</v>
       </c>
       <c r="B8">
-        <v>5.572222</v>
+        <v>0.51111119999999999</v>
       </c>
       <c r="C8">
-        <v>-7.3577779999999997</v>
+        <v>-9.9533330000000007</v>
       </c>
       <c r="D8">
-        <v>0.7899969</v>
+        <f t="shared" si="0"/>
+        <v>0.70072400000000001</v>
       </c>
       <c r="E8">
-        <f t="shared" si="0"/>
-        <v>-6.9994137672899817E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.93693596653799971</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
-        <v>4.5141572176859084</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0.6124029642991502</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7999411</v>
+        <v>800230</v>
       </c>
       <c r="B9">
-        <v>6.1644439999999996</v>
+        <v>1.39</v>
       </c>
       <c r="C9">
-        <v>-5.3533330000000001</v>
+        <v>-7.5811109999999999</v>
       </c>
       <c r="D9">
-        <v>0.79994109999999996</v>
+        <f t="shared" si="0"/>
+        <v>0.80023</v>
       </c>
       <c r="E9">
-        <f t="shared" si="0"/>
-        <v>-6.3200915003099725E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.87239119233199991</v>
       </c>
       <c r="F9">
-        <f t="shared" si="1"/>
-        <v>4.4509563026828083</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <f>MOD(E9+F8, 2*PI())</f>
+        <v>1.4847941566311502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>8099699</v>
+        <v>900793</v>
       </c>
       <c r="B10">
-        <v>0.28444439999999999</v>
+        <v>2.0477780000000001</v>
       </c>
       <c r="C10">
-        <v>-3.4866670000000002</v>
+        <v>-4.9411110000000003</v>
       </c>
       <c r="D10">
-        <v>0.80996990000000002</v>
+        <f t="shared" si="0"/>
+        <v>0.90079299999999995</v>
       </c>
       <c r="E10">
-        <f t="shared" si="0"/>
-        <v>-4.4327296000000266E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.62963610549299975</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
-        <v>4.4066290066828078</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.11443026212415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>8199966</v>
+        <v>900793</v>
       </c>
       <c r="B11">
-        <v>0.64444449999999998</v>
+        <v>2.0477780000000001</v>
       </c>
       <c r="C11">
-        <v>-4.1644439999999996</v>
+        <v>-4.9411110000000003</v>
       </c>
       <c r="D11">
-        <v>0.81999659999999996</v>
+        <f t="shared" si="0"/>
+        <v>0.90079299999999995</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
-        <v>-3.8357697331849787E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
-        <v>4.3682713093509582</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.11443026212415</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>8299551</v>
+        <v>1001812</v>
       </c>
       <c r="B12">
-        <v>1.0511109999999999</v>
+        <v>2.423333</v>
       </c>
       <c r="C12">
-        <v>-4.3533330000000001</v>
+        <v>-4.4244450000000004</v>
       </c>
       <c r="D12">
-        <v>0.82995509999999995</v>
+        <f t="shared" si="0"/>
+        <v>1.0018119999999999</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
-        <v>-4.2412141127249912E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.47304955078199995</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
-        <v>4.3258591682237082</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2.58747981290615</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>8399968</v>
+        <v>1200251</v>
       </c>
       <c r="B13">
-        <v>1.4388890000000001</v>
+        <v>3.2455560000000001</v>
       </c>
       <c r="C13">
-        <v>-3.8011110000000001</v>
+        <v>-4.2544449999999996</v>
       </c>
       <c r="D13">
-        <v>0.83999679999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.200251</v>
       </c>
       <c r="E13">
-        <f t="shared" si="0"/>
-        <v>-4.0942240157400174E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.86111512635500009</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
-        <v>4.2849169280663082</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>3.4485949392611501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>8499569</v>
+        <v>1300329</v>
       </c>
       <c r="B14">
-        <v>1.8011109999999999</v>
+        <v>3.6422219999999998</v>
       </c>
       <c r="C14">
-        <v>-3.8822220000000001</v>
+        <v>-4.032222</v>
       </c>
       <c r="D14">
-        <v>0.84995690000000002</v>
+        <f t="shared" si="0"/>
+        <v>1.3003290000000001</v>
       </c>
       <c r="E14">
-        <f t="shared" si="0"/>
-        <v>-3.8263382506650102E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.41465653001300046</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
-        <v>4.2466535455596581</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>3.8632514692741506</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>8599946</v>
+        <v>1400241</v>
       </c>
       <c r="B15">
-        <v>2.1755550000000001</v>
+        <v>4.0122220000000004</v>
       </c>
       <c r="C15">
-        <v>-3.9822220000000002</v>
+        <v>-3.7644440000000001</v>
       </c>
       <c r="D15">
-        <v>0.85999460000000005</v>
+        <f t="shared" si="0"/>
+        <v>1.4002410000000001</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
-        <v>-3.9470464769400151E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.38949024669600002</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
-        <v>4.2071830807902577</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.252741715970151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>8700346</v>
+        <v>1500226</v>
       </c>
       <c r="B16">
-        <v>2.5511110000000001</v>
+        <v>4.3633329999999999</v>
       </c>
       <c r="C16">
-        <v>-3.697778</v>
+        <v>-3.661111</v>
       </c>
       <c r="D16">
-        <v>0.87003459999999999</v>
+        <f t="shared" si="0"/>
+        <v>1.5002260000000001</v>
       </c>
       <c r="E16">
-        <f t="shared" si="0"/>
-        <v>-3.8553599999999758E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.37122205833749999</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
-        <v>4.1686294807902575</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.6239637743076507</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>8799919</v>
+        <v>1500226</v>
       </c>
       <c r="B17">
+        <v>4.3633329999999999</v>
+      </c>
+      <c r="C17">
+        <v>-3.661111</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1.5002260000000001</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="2"/>
+        <v>4.6239637743076507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1700789</v>
+      </c>
+      <c r="B18">
+        <v>5.0766669999999996</v>
+      </c>
+      <c r="C18">
+        <v>-3.8044449999999999</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.7007890000000001</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>0.74865715401400013</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>5.3726209283216511</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1800879</v>
+      </c>
+      <c r="B19">
+        <v>5.4377779999999998</v>
+      </c>
+      <c r="C19">
+        <v>-3.8411110000000002</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1.8008789999999999</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>0.38262185001999921</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="2"/>
+        <v>5.7552427783416507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1900234</v>
+      </c>
+      <c r="B20">
+        <v>5.7977780000000001</v>
+      </c>
+      <c r="C20">
+        <v>-3.6688890000000001</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.900234</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>0.37307802500000031</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>6.1283208033416514</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>2000486</v>
+      </c>
+      <c r="B21">
+        <v>6.14</v>
+      </c>
+      <c r="C21">
+        <v>-3.52</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>2.000486</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>0.36035025001400001</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="2"/>
+        <v>0.2054857461760653</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>2100548</v>
+      </c>
+      <c r="B22">
+        <v>0.24444440000000001</v>
+      </c>
+      <c r="C22">
+        <v>-3.8144450000000001</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>2.1005479999999999</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>0.36694961779499957</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="2"/>
+        <v>0.57243536397106487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>2100548</v>
+      </c>
+      <c r="B23">
+        <v>0.24444440000000001</v>
+      </c>
+      <c r="C23">
+        <v>-3.8144450000000001</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>2.1005479999999999</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="2"/>
+        <v>0.57243536397106487</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>2300694</v>
+      </c>
+      <c r="B24">
+        <v>0.92222219999999999</v>
+      </c>
+      <c r="C24">
+        <v>-3.62</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2.300694</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>0.7439872144850006</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="2"/>
+        <v>1.3164225784560655</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2400541</v>
+      </c>
+      <c r="B25">
+        <v>1.263333</v>
+      </c>
+      <c r="C25">
+        <v>-3.6344439999999998</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>2.400541</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>0.36216723503400006</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>1.6785898134900656</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>2500562</v>
+      </c>
+      <c r="B26">
+        <v>1.611111</v>
+      </c>
+      <c r="C26">
+        <v>-3.6311110000000002</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2.500562</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>0.36335403832749968</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>2.0419438518175652</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>2600665</v>
+      </c>
+      <c r="B27">
+        <v>1.947778</v>
+      </c>
+      <c r="C27">
+        <v>-3.4466670000000001</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>2.6006649999999998</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>0.35425340556699941</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>2.3961972573845647</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>2700837</v>
+      </c>
+      <c r="B28">
+        <v>2.2844440000000001</v>
+      </c>
+      <c r="C28">
+        <v>-3.661111</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2.7008369999999999</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>0.35600016890800051</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>2.752197426292565</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>2800410</v>
+      </c>
+      <c r="B29">
+        <v>2.6433330000000002</v>
+      </c>
+      <c r="C29">
+        <v>-3.851111</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2.8004099999999998</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>0.37400724060299967</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>3.1262046668955645</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>2800410</v>
+      </c>
+      <c r="B30">
+        <v>2.6433330000000002</v>
+      </c>
+      <c r="C30">
+        <v>-3.851111</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>2.8004099999999998</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="2"/>
+        <v>3.1262046668955645</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3000208</v>
+      </c>
+      <c r="B31">
+        <v>3.342222</v>
+      </c>
+      <c r="C31">
+        <v>-3.6044450000000001</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3.0002080000000002</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>0.7448025888440013</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>3.8710072557395661</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>3000208</v>
+      </c>
+      <c r="B32">
+        <v>3.342222</v>
+      </c>
+      <c r="C32">
+        <v>-3.6044450000000001</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3.0002080000000002</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>3.8710072557395661</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>3101803</v>
+      </c>
+      <c r="B33">
+        <v>3.69</v>
+      </c>
+      <c r="C33">
+        <v>-3.6755550000000001</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>3.1018029999999999</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>0.36980579999999874</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>4.2408130557395651</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3311946</v>
+      </c>
+      <c r="B34">
+        <v>4.4288889999999999</v>
+      </c>
+      <c r="C34">
+        <v>-3.7588889999999999</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>3.3119459999999998</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>0.78114818274599984</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>5.0219612384855647</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>3400574</v>
+      </c>
+      <c r="B35">
+        <v>4.7033329999999998</v>
+      </c>
+      <c r="C35">
+        <v>-3.5344440000000001</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>3.4005740000000002</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>0.32319675856200136</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>5.3451579970475658</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>3500374</v>
+      </c>
+      <c r="B36">
+        <v>5.0422219999999998</v>
+      </c>
+      <c r="C36">
+        <v>-3.5755560000000002</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>3.5003739999999999</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>0.35478899999999886</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>5.6999469970475642</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>3600620</v>
+      </c>
+      <c r="B37">
+        <v>5.39</v>
+      </c>
+      <c r="C37">
+        <v>-3.8055560000000002</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>3.6006200000000002</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>0.369963476776001</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>6.0699104738235654</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>3700346</v>
+      </c>
+      <c r="B38">
+        <v>5.7444439999999997</v>
+      </c>
+      <c r="C38">
+        <v>-3.6666669999999999</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>3.7003460000000001</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>0.3725874554489999</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>0.15931262209297881</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>3800523</v>
+      </c>
+      <c r="B39">
+        <v>6.0944440000000002</v>
+      </c>
+      <c r="C39">
+        <v>-3.84</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>3.8005230000000001</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>0.37599769002949984</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>0.5353103121224787</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>3900758</v>
+      </c>
+      <c r="B40">
+        <v>0.17222219999999999</v>
+      </c>
+      <c r="C40">
+        <v>-3.6677780000000002</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>3.9007580000000002</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>0.37627106391500026</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>0.91158137603747891</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>4000778</v>
+      </c>
+      <c r="B41">
+        <v>0.51444440000000002</v>
+      </c>
+      <c r="C41">
+        <v>-3.51</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>4.0007780000000004</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>0.35896067778000079</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>1.2705420538174796</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>4000778</v>
+      </c>
+      <c r="B42">
+        <v>0.51444440000000002</v>
+      </c>
+      <c r="C42">
+        <v>-3.51</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>4.0007780000000004</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>1.2705420538174796</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>4200570</v>
+      </c>
+      <c r="B43">
+        <v>1.2144440000000001</v>
+      </c>
+      <c r="C43">
+        <v>-3.7422219999999999</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>4.2005699999999999</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>0.72446796891199827</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>1.995010022729478</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>4300807</v>
+      </c>
+      <c r="B44">
+        <v>1.562222</v>
+      </c>
+      <c r="C44">
+        <v>-3.523333</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>4.3008069999999998</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>0.36413871826749966</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>2.3591487409969778</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>4400390</v>
+      </c>
+      <c r="B45">
+        <v>1.9044449999999999</v>
+      </c>
+      <c r="C45">
+        <v>-3.6911109999999998</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>4.4003899999999998</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>0.35921798842599995</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="2"/>
+        <v>2.7183667294229776</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>4500552</v>
+      </c>
+      <c r="B46">
+        <v>2.25</v>
+      </c>
+      <c r="C46">
+        <v>-3.5344440000000001</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>4.5005519999999999</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>0.36186301995500031</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="2"/>
+        <v>3.080229749377978</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>4600392</v>
+      </c>
+      <c r="B47">
+        <v>2.5911110000000002</v>
+      </c>
+      <c r="C47">
+        <v>-3.664444</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>4.6003920000000003</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>0.35936848896000134</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="2"/>
+        <v>3.4395982383379793</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>4700672</v>
+      </c>
+      <c r="B48">
         <v>2.943333</v>
       </c>
-      <c r="C17">
-        <v>-3.8655560000000002</v>
-      </c>
-      <c r="D17">
-        <v>0.87999190000000005</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>-3.7655192819100222E-2</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>4.1309742879711573</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>8899638</v>
-      </c>
-      <c r="B18">
-        <v>3.2766670000000002</v>
-      </c>
-      <c r="C18">
-        <v>-3.8633329999999999</v>
-      </c>
-      <c r="D18">
-        <v>0.88996379999999997</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>-3.8535854109549704E-2</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
-        <v>4.0924384338616075</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>8999820</v>
-      </c>
-      <c r="B19">
-        <v>3.637778</v>
-      </c>
-      <c r="C19">
-        <v>-3.66</v>
-      </c>
-      <c r="D19">
-        <v>0.89998199999999995</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>-3.7685127330299911E-2</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
-        <v>4.0547533065313077</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>9100071</v>
-      </c>
-      <c r="B20">
-        <v>3.9944440000000001</v>
-      </c>
-      <c r="C20">
-        <v>-3.7688890000000002</v>
-      </c>
-      <c r="D20">
-        <v>0.91000709999999996</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>-3.7237677556950032E-2</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>4.0175156289743574</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>9200152</v>
-      </c>
-      <c r="B21">
-        <v>4.3411109999999997</v>
-      </c>
-      <c r="C21">
-        <v>-3.6</v>
-      </c>
-      <c r="D21">
-        <v>0.92001520000000003</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>-3.6874289000450276E-2</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>3.9806413399739071</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>9299987</v>
-      </c>
-      <c r="B22">
-        <v>4.6822220000000003</v>
-      </c>
-      <c r="C22">
-        <v>-3.67</v>
-      </c>
-      <c r="D22">
-        <v>0.92999869999999996</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>-3.629002249999972E-2</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
-        <v>3.9443513174739073</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>9400339</v>
-      </c>
-      <c r="B23">
-        <v>5.032222</v>
-      </c>
-      <c r="C23">
-        <v>-3.7966669999999998</v>
-      </c>
-      <c r="D23">
-        <v>0.94003389999999998</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>-3.7464748339200077E-2</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="1"/>
-        <v>3.9068865691347074</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>9499893</v>
-      </c>
-      <c r="B24">
-        <v>5.3911110000000004</v>
-      </c>
-      <c r="C24">
-        <v>-3.75</v>
-      </c>
-      <c r="D24">
-        <v>0.94998930000000004</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>-3.7565044325900215E-2</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="1"/>
-        <v>3.8693215248088073</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>9600307</v>
-      </c>
-      <c r="B25">
-        <v>5.7711110000000003</v>
-      </c>
-      <c r="C25">
-        <v>-3.53</v>
-      </c>
-      <c r="D25">
-        <v>0.96003070000000001</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>-3.6550695999999917E-2</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="1"/>
-        <v>3.8327708288088074</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>9699746</v>
-      </c>
-      <c r="B26">
-        <v>6.0733329999999999</v>
-      </c>
-      <c r="C26">
-        <v>-3.5555560000000002</v>
-      </c>
-      <c r="D26">
-        <v>0.96997460000000002</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>-3.5229030154200022E-2</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="1"/>
-        <v>3.7975417986546072</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9800033</v>
-      </c>
-      <c r="B27">
-        <v>0.1366667</v>
-      </c>
-      <c r="C27">
-        <v>-3.7444440000000001</v>
-      </c>
-      <c r="D27">
-        <v>0.98000330000000002</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>-3.660475500000001E-2</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="1"/>
-        <v>3.7609370436546072</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>9899649</v>
-      </c>
-      <c r="B28">
-        <v>0.48333330000000002</v>
-      </c>
-      <c r="C28">
-        <v>-3.56</v>
-      </c>
-      <c r="D28">
-        <v>0.98996490000000004</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>-3.6381974675200053E-2</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
-        <v>3.7245550689794071</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>9998537</v>
-      </c>
-      <c r="B29">
-        <v>0.82555559999999995</v>
-      </c>
-      <c r="C29">
-        <v>-3.6888890000000001</v>
-      </c>
-      <c r="D29">
-        <v>0.99985369999999996</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>-3.5841406771599707E-2</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="1"/>
-        <v>3.6887136622078076</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>10099913</v>
-      </c>
-      <c r="B30">
-        <v>1.1822220000000001</v>
-      </c>
-      <c r="C30">
-        <v>-3.7433329999999998</v>
-      </c>
-      <c r="D30">
-        <v>1.0099913</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>-3.7672446873600295E-2</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="1"/>
-        <v>3.6510412153342071</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>10199444</v>
-      </c>
-      <c r="B31">
-        <v>1.5377780000000001</v>
-      </c>
-      <c r="C31">
-        <v>-3.6866669999999999</v>
-      </c>
-      <c r="D31">
-        <v>1.0199444</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>-3.6975766499999764E-2</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="1"/>
-        <v>3.6140654488342072</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>10299885</v>
-      </c>
-      <c r="B32">
-        <v>1.8833329999999999</v>
-      </c>
-      <c r="C32">
-        <v>-3.5444450000000001</v>
-      </c>
-      <c r="D32">
-        <v>1.0299885</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>-3.6315006019599999E-2</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
-        <v>3.5777504428146072</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>10399650</v>
-      </c>
-      <c r="B33">
-        <v>2.2255560000000001</v>
-      </c>
-      <c r="C33">
-        <v>-3.6322220000000001</v>
-      </c>
-      <c r="D33">
-        <v>1.039965</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>-3.5799009162750195E-2</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="1"/>
-        <v>3.5419514336518572</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>10499559</v>
-      </c>
-      <c r="B34">
-        <v>2.5733329999999999</v>
-      </c>
-      <c r="C34">
-        <v>-3.6633330000000002</v>
-      </c>
-      <c r="D34">
-        <v>1.0499559000000001</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>-3.6444580224750091E-2</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="1"/>
-        <v>3.5055068534271072</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>10599941</v>
-      </c>
-      <c r="B35">
-        <v>2.9344440000000001</v>
-      </c>
-      <c r="C35">
-        <v>-3.8777780000000002</v>
-      </c>
-      <c r="D35">
-        <v>1.0599940999999999</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>-3.7849590220099573E-2</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
-        <v>3.4676572632070077</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>10700308</v>
-      </c>
-      <c r="B36">
-        <v>3.2966669999999998</v>
-      </c>
-      <c r="C36">
-        <v>-3.6066669999999998</v>
-      </c>
-      <c r="D36">
-        <v>1.0700308000000001</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>-3.755956456575045E-2</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="1"/>
-        <v>3.4300976986412572</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>10799960</v>
-      </c>
-      <c r="B37">
-        <v>3.6677780000000002</v>
-      </c>
-      <c r="C37">
-        <v>-3.4922219999999999</v>
-      </c>
-      <c r="D37">
-        <v>1.079996</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>-3.5370924331399628E-2</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="1"/>
-        <v>3.3947267743098575</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>10899581</v>
-      </c>
-      <c r="B38">
-        <v>3.9377779999999998</v>
-      </c>
-      <c r="C38">
-        <v>-3.673333</v>
-      </c>
-      <c r="D38">
-        <v>1.0899581</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>-3.5691987732750299E-2</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="1"/>
-        <v>3.3590347865771073</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>10999858</v>
-      </c>
-      <c r="B39">
-        <v>4.29</v>
-      </c>
-      <c r="C39">
-        <v>-3.5944449999999999</v>
-      </c>
-      <c r="D39">
-        <v>1.0999858</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>-3.6439548725299899E-2</v>
-      </c>
-      <c r="F39">
-        <f t="shared" si="1"/>
-        <v>3.3225952378518073</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>11099412</v>
-      </c>
-      <c r="B40">
-        <v>4.6355560000000002</v>
-      </c>
-      <c r="C40">
-        <v>-3.6422219999999998</v>
-      </c>
-      <c r="D40">
-        <v>1.1099412</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>-3.6021957325899807E-2</v>
-      </c>
-      <c r="F40">
-        <f t="shared" si="1"/>
-        <v>3.2865732805259076</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>11199737</v>
-      </c>
-      <c r="B41">
-        <v>4.9822220000000002</v>
-      </c>
-      <c r="C41">
-        <v>-3.6477780000000002</v>
-      </c>
-      <c r="D41">
-        <v>1.1199737000000001</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>-3.6568462500000405E-2</v>
-      </c>
-      <c r="F41">
-        <f t="shared" si="1"/>
-        <v>3.2500048180259071</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>11300136</v>
-      </c>
-      <c r="B42">
-        <v>5.3288890000000002</v>
-      </c>
-      <c r="C42">
-        <v>-3.6533329999999999</v>
-      </c>
-      <c r="D42">
-        <v>1.1300136000000001</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>-3.665121216444997E-2</v>
-      </c>
-      <c r="F42">
-        <f t="shared" si="1"/>
-        <v>3.2133536058614571</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>11400154</v>
-      </c>
-      <c r="B43">
-        <v>5.6733330000000004</v>
-      </c>
-      <c r="C43">
-        <v>-3.5577779999999999</v>
-      </c>
-      <c r="D43">
-        <v>1.1400154</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>-3.6062044999899817E-2</v>
-      </c>
-      <c r="F43">
-        <f t="shared" si="1"/>
-        <v>3.1772915608615575</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>11500373</v>
-      </c>
-      <c r="B44">
-        <v>6.016667</v>
-      </c>
-      <c r="C44">
-        <v>-3.7311109999999998</v>
-      </c>
-      <c r="D44">
-        <v>1.1500372999999999</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>-3.652425833454969E-2</v>
-      </c>
-      <c r="F44">
-        <f t="shared" si="1"/>
-        <v>3.1407673025270078</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>11600511</v>
-      </c>
-      <c r="B45">
-        <v>0.1244444</v>
-      </c>
-      <c r="C45">
-        <v>-3.7455560000000001</v>
-      </c>
-      <c r="D45">
-        <v>1.1600511</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>-3.7434924002300272E-2</v>
-      </c>
-      <c r="F45">
-        <f t="shared" si="1"/>
-        <v>3.1033323785247076</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>11699215</v>
-      </c>
-      <c r="B46">
-        <v>0.1244444</v>
-      </c>
-      <c r="C46">
-        <v>-3.7455560000000001</v>
-      </c>
-      <c r="D46">
-        <v>1.1699215000000001</v>
-      </c>
-      <c r="E46">
-        <f t="shared" si="0"/>
-        <v>-3.6970135942400215E-2</v>
-      </c>
-      <c r="F46">
-        <f t="shared" si="1"/>
-        <v>3.0663622425823074</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>11799693</v>
-      </c>
-      <c r="B47">
-        <v>0.79222219999999999</v>
-      </c>
-      <c r="C47">
-        <v>-3.5666669999999998</v>
-      </c>
-      <c r="D47">
-        <v>1.1799693</v>
-      </c>
-      <c r="E47">
-        <f t="shared" si="0"/>
-        <v>-3.6735877129699779E-2</v>
-      </c>
-      <c r="F47">
-        <f t="shared" si="1"/>
-        <v>3.0296263654526077</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>11899913</v>
-      </c>
-      <c r="B48">
-        <v>1.131111</v>
-      </c>
       <c r="C48">
-        <v>-3.5677780000000001</v>
+        <v>-3.6622219999999999</v>
       </c>
       <c r="D48">
-        <v>1.1899913</v>
+        <f t="shared" si="0"/>
+        <v>4.700672</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
-        <v>-3.5750703894999909E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.36735903323999891</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
-        <v>2.9938756615576079</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>3.806957271577978</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>11999192</v>
+        <v>4800630</v>
       </c>
       <c r="B49">
-        <v>1.4744440000000001</v>
+        <v>3.3277779999999999</v>
       </c>
       <c r="C49">
-        <v>-3.6022219999999998</v>
+        <v>-3.6911109999999998</v>
       </c>
       <c r="D49">
-        <v>1.1999192000000001</v>
+        <f t="shared" si="0"/>
+        <v>4.80063</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
-        <v>-3.5591521500000362E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.36751223000699995</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
-        <v>2.9582841400576076</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.1744695015849782</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>12099815</v>
+        <v>4900709</v>
       </c>
       <c r="B50">
-        <v>1.828889</v>
+        <v>3.641111</v>
       </c>
       <c r="C50">
-        <v>-3.806667</v>
+        <v>-3.6466669999999999</v>
       </c>
       <c r="D50">
-        <v>1.2099815</v>
+        <f t="shared" si="0"/>
+        <v>4.900709</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
-        <v>-3.7275231892349887E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.36717874223100011</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
-        <v>2.9210089081652577</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.5416482438159784</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>12200139</v>
+        <v>5000575</v>
       </c>
       <c r="B51">
-        <v>2.1844440000000001</v>
+        <v>3.99</v>
       </c>
       <c r="C51">
-        <v>-3.6188889999999998</v>
+        <v>-3.7088890000000001</v>
       </c>
       <c r="D51">
-        <v>1.2200139000000001</v>
+        <f t="shared" si="0"/>
+        <v>5.0005750000000004</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
-        <v>-3.7248074007200198E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.36728497774800167</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
-        <v>2.8837608341580574</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>4.9089332215639798</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>12299788</v>
+        <v>5100567</v>
       </c>
       <c r="B52">
-        <v>2.5311110000000001</v>
+        <v>4.3355560000000004</v>
       </c>
       <c r="C52">
-        <v>-3.7166670000000002</v>
+        <v>-3.5533329999999999</v>
       </c>
       <c r="D52">
-        <v>1.2299788</v>
+        <f t="shared" si="0"/>
+        <v>5.1005669999999999</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
-        <v>-3.6549040992199792E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.36308205111199787</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
-        <v>2.8472117931658576</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>5.2720152726759775</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>12399539</v>
+        <v>5200616</v>
       </c>
       <c r="B53">
-        <v>2.8844439999999998</v>
+        <v>4.6722219999999997</v>
       </c>
       <c r="C53">
-        <v>-3.677778</v>
+        <v>-3.6355559999999998</v>
       </c>
       <c r="D53">
-        <v>1.2399538999999999</v>
+        <f t="shared" si="0"/>
+        <v>5.2006160000000001</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
-        <v>-3.6880164159749644E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.35962057778050099</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
-        <v>2.8103316290061078</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>5.6316358504564787</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>12500240</v>
+        <v>5300739</v>
       </c>
       <c r="B54">
-        <v>3.2388889999999999</v>
+        <v>5.0244450000000001</v>
       </c>
       <c r="C54">
-        <v>-3.7033330000000002</v>
+        <v>-3.77</v>
       </c>
       <c r="D54">
-        <v>1.250024</v>
+        <f t="shared" si="0"/>
+        <v>5.3007390000000001</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
-        <v>-3.7164262940550308E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.37073324169399985</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
-        <v>2.7731673660655574</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>12599834</v>
-      </c>
-      <c r="B55">
-        <v>3.585556</v>
-      </c>
-      <c r="C55">
-        <v>-3.5388890000000002</v>
-      </c>
-      <c r="D55">
-        <v>1.2599834000000001</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>6.0023690921504782</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E55">
-        <f t="shared" si="0"/>
-        <v>-3.6064092893400228E-2</v>
-      </c>
-      <c r="F55">
-        <f t="shared" si="1"/>
-        <v>2.7371032731721572</v>
+        <f t="shared" si="1"/>
+        <v>-9.9918930150000005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>